<commit_message>
update code and bonneville spawners
</commit_message>
<xml_diff>
--- a/updated_data/brood_tables_raw/COLUMBIA_Sockeye age comp at Bon all years.xlsx
+++ b/updated_data/brood_tables_raw/COLUMBIA_Sockeye age comp at Bon all years.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\PIT tag analysis\All years work\Sockeye Analyses\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haleyoleynik/Documents/GitHub/salmon-prize_2024/updated_data/brood_tables_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CFF6E2F-24B8-44BA-96E7-C86D8C2B3703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E325A2DF-571F-9048-AEE1-DE2296CF1AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24195" yWindow="-15720" windowWidth="38130" windowHeight="14385" xr2:uid="{DE3544A4-0BAC-455E-9AF0-F54481F8261B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{DE3544A4-0BAC-455E-9AF0-F54481F8261B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -95,9 +95,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,7 +135,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -241,7 +241,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,7 +383,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95CF3C2-F983-461B-8D9B-2509F74BDFBC}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +437,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>166340</v>
       </c>
@@ -477,8 +477,12 @@
       <c r="M2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="1">
+        <f>SUM(C2:M2)</f>
+        <v>166340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>58123</v>
       </c>
@@ -519,7 +523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>116993</v>
       </c>
@@ -560,7 +564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>79714</v>
       </c>
@@ -601,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>41884</v>
       </c>
@@ -642,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>49581</v>
       </c>
@@ -683,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>76481</v>
       </c>
@@ -724,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>84992</v>
       </c>
@@ -765,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>80178</v>
       </c>
@@ -806,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>12678</v>
       </c>
@@ -847,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8774</v>
       </c>
@@ -888,7 +892,7 @@
         <v>41.203706057140096</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>30232</v>
       </c>
@@ -929,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>47008</v>
       </c>
@@ -970,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13218</v>
       </c>
@@ -1011,7 +1015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>17877</v>
       </c>
@@ -1052,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>93398</v>
       </c>
@@ -1093,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>114934</v>
       </c>
@@ -1134,7 +1138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>49610</v>
       </c>
@@ -1175,7 +1179,7 @@
         <v>190.62716206430562</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>39291</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>123291</v>
       </c>
@@ -1257,7 +1261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>72971</v>
       </c>
@@ -1298,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>37066</v>
       </c>
@@ -1339,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>24376</v>
       </c>
@@ -1380,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>213607</v>
       </c>
@@ -1421,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>177823</v>
       </c>
@@ -1462,7 +1466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>386525</v>
       </c>
@@ -1503,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>185796</v>
       </c>
@@ -1544,7 +1548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>515673</v>
       </c>
@@ -1585,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>185505</v>
       </c>
@@ -1626,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>614179</v>
       </c>
@@ -1667,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>510706</v>
       </c>
@@ -1708,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>342498</v>
       </c>
@@ -1749,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>87693</v>
       </c>
@@ -1790,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>193816</v>
       </c>
@@ -1831,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>63046</v>
       </c>
@@ -1872,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>341739</v>
       </c>
@@ -1913,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>151765</v>
       </c>
@@ -1954,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>663253</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>327600</v>
       </c>

</xml_diff>